<commit_message>
2021-04-28 JCS : Mise à jour titre lettre
</commit_message>
<xml_diff>
--- a/FulOverdueAndLostLoanNotificationLetter/FulOverdueAndLostLoanNotificationLetter-param-french.xlsx
+++ b/FulOverdueAndLostLoanNotificationLetter/FulOverdueAndLostLoanNotificationLetter-param-french.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="rowsForView" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
     <t>Long Overdue Items - Notification</t>
   </si>
   <si>
-    <t>Lettre de relance - 2e rappel</t>
+    <t>Lettre de relance - dernier rappel</t>
   </si>
   <si>
     <t>subject</t>
@@ -1194,7 +1194,7 @@
         <v>20</v>
       </c>
       <c r="F25" s="1">
-        <v>44307</v>
+        <v>44314</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>20</v>
       </c>
       <c r="F26" s="1">
-        <v>44307</v>
+        <v>44314</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
2021-07-21 JCS : mise à jour paramétrage
</commit_message>
<xml_diff>
--- a/FulOverdueAndLostLoanNotificationLetter/FulOverdueAndLostLoanNotificationLetter-param-french.xlsx
+++ b/FulOverdueAndLostLoanNotificationLetter/FulOverdueAndLostLoanNotificationLetter-param-french.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="112">
   <si>
     <t>Activé</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>additional_info_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due to the health context, an appointment is required. You can select a time slot here: </t>
   </si>
   <si>
     <t>En raison du contexte sanitaire, la prise de rendez-vous est obligatoire. Vous pouvez sélectionner un créneau en suivant ce lien :</t>
@@ -689,7 +686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -865,16 +864,16 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="1">
-        <v>44307</v>
+        <v>44379</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,13 +881,13 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -902,13 +901,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -922,13 +921,13 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -942,13 +941,13 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -962,13 +961,13 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -982,13 +981,13 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1002,13 +1001,13 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1022,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1042,13 +1041,13 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1062,13 +1061,13 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1082,13 +1081,13 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1102,13 +1101,13 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>10</v>
@@ -1122,13 +1121,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -1142,13 +1141,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
@@ -1162,13 +1161,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
       </c>
       <c r="E24" t="s">
         <v>10</v>
@@ -1182,13 +1181,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
         <v>55</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>56</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
@@ -1202,13 +1201,13 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
         <v>56</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
       </c>
       <c r="E26" t="s">
         <v>20</v>
@@ -1222,13 +1221,13 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>60</v>
-      </c>
-      <c r="D27" t="s">
-        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>10</v>
@@ -1242,13 +1241,13 @@
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
         <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
       </c>
       <c r="E28" t="s">
         <v>10</v>
@@ -1262,13 +1261,13 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
         <v>63</v>
       </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
         <v>10</v>
@@ -1282,13 +1281,13 @@
         <v>6</v>
       </c>
       <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>66</v>
-      </c>
-      <c r="D30" t="s">
-        <v>67</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
@@ -1302,13 +1301,13 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>69</v>
-      </c>
-      <c r="D31" t="s">
-        <v>70</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1322,13 +1321,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
         <v>71</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>72</v>
-      </c>
-      <c r="D32" t="s">
-        <v>73</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -1342,13 +1341,13 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
         <v>74</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>75</v>
-      </c>
-      <c r="D33" t="s">
-        <v>76</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -1362,13 +1361,13 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
         <v>77</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>78</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
       </c>
       <c r="E34" t="s">
         <v>20</v>
@@ -1382,13 +1381,13 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
         <v>80</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>81</v>
-      </c>
-      <c r="D35" t="s">
-        <v>82</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1402,13 +1401,13 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
         <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" t="s">
-        <v>84</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
@@ -1422,13 +1421,13 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
         <v>85</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>86</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
@@ -1442,13 +1441,13 @@
         <v>6</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
@@ -1462,13 +1461,13 @@
         <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
         <v>81</v>
-      </c>
-      <c r="D39" t="s">
-        <v>82</v>
       </c>
       <c r="E39" t="s">
         <v>10</v>
@@ -1482,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" t="s">
         <v>81</v>
-      </c>
-      <c r="D40" t="s">
-        <v>82</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
@@ -1502,13 +1501,13 @@
         <v>6</v>
       </c>
       <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
         <v>91</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>92</v>
-      </c>
-      <c r="D41" t="s">
-        <v>93</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
@@ -1522,13 +1521,13 @@
         <v>6</v>
       </c>
       <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" t="s">
         <v>94</v>
       </c>
-      <c r="C42" t="s">
-        <v>95</v>
-      </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1542,13 +1541,13 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s">
         <v>10</v>
@@ -1562,13 +1561,13 @@
         <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
         <v>10</v>
@@ -1582,13 +1581,13 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
         <v>10</v>
@@ -1602,13 +1601,13 @@
         <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s">
         <v>10</v>
@@ -1622,13 +1621,13 @@
         <v>6</v>
       </c>
       <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
         <v>100</v>
       </c>
-      <c r="C47" t="s">
-        <v>101</v>
-      </c>
       <c r="D47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
@@ -1642,13 +1641,13 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
         <v>102</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>103</v>
-      </c>
-      <c r="D48" t="s">
-        <v>104</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -1662,13 +1661,13 @@
         <v>6</v>
       </c>
       <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" t="s">
         <v>105</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>106</v>
-      </c>
-      <c r="D49" t="s">
-        <v>107</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -1682,13 +1681,13 @@
         <v>6</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" t="s">
         <v>106</v>
-      </c>
-      <c r="D50" t="s">
-        <v>107</v>
       </c>
       <c r="E50" t="s">
         <v>10</v>
@@ -1702,13 +1701,13 @@
         <v>6</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
         <v>106</v>
-      </c>
-      <c r="D51" t="s">
-        <v>107</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
@@ -1722,13 +1721,13 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" t="s">
         <v>106</v>
-      </c>
-      <c r="D52" t="s">
-        <v>107</v>
       </c>
       <c r="E52" t="s">
         <v>10</v>
@@ -1742,13 +1741,13 @@
         <v>6</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" t="s">
         <v>106</v>
-      </c>
-      <c r="D53" t="s">
-        <v>107</v>
       </c>
       <c r="E53" t="s">
         <v>10</v>
@@ -1762,13 +1761,13 @@
         <v>6</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" t="s">
         <v>106</v>
-      </c>
-      <c r="D54" t="s">
-        <v>107</v>
       </c>
       <c r="E54" t="s">
         <v>10</v>

</xml_diff>